<commit_message>
Checkpoint after Skype Call Plot for global fit is not working Need to add names of global variable to the list of items that can be enterd. Need to create a default constants file.
</commit_message>
<xml_diff>
--- a/Fits/fit_results.xlsx
+++ b/Fits/fit_results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Control File</t>
   </si>
@@ -42,22 +42,82 @@
     <t>W</t>
   </si>
   <si>
+    <t>Tmin</t>
+  </si>
+  <si>
+    <t>Tmax</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Yscale</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
     <t>stderr</t>
   </si>
   <si>
+    <t>Fit001</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>ERF</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Sven&amp; Quan E0=1.68 W=.372</t>
+  </si>
+  <si>
+    <t>Fit002</t>
+  </si>
+  <si>
+    <t>Fit003</t>
+  </si>
+  <si>
+    <t>Fit004</t>
+  </si>
+  <si>
+    <t>Fit005</t>
+  </si>
+  <si>
+    <t>Fit006</t>
+  </si>
+  <si>
+    <t>Fit007</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Fit008</t>
+  </si>
+  <si>
+    <t>Fit009</t>
+  </si>
+  <si>
     <t>Fit010</t>
   </si>
   <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>ERF</t>
-  </si>
-  <si>
-    <t>None</t>
+    <t>Fit011</t>
+  </si>
+  <si>
+    <t>Fit013</t>
+  </si>
+  <si>
+    <t>Fit014</t>
+  </si>
+  <si>
+    <t>Fit015</t>
   </si>
 </sst>
 </file>
@@ -98,33 +158,33 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -429,10 +489,10 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -441,135 +501,705 @@
     <col customWidth="1" max="2" min="2" style="9" width="9.140625"/>
     <col customWidth="1" max="3" min="3" style="9" width="4.140625"/>
     <col customWidth="1" max="4" min="4" style="9" width="2.85546875"/>
-    <col customWidth="1" max="5" min="5" style="10" width="8.7109375"/>
-    <col customWidth="1" max="6" min="6" style="10" width="10.42578125"/>
-    <col customWidth="1" max="9" min="7" style="7" width="8.7109375"/>
-    <col customWidth="1" max="9" min="7" style="7" width="8.7109375"/>
-    <col customWidth="1" max="9" min="7" style="7" width="8.7109375"/>
+    <col customWidth="1" max="5" min="5" style="2" width="8.7109375"/>
+    <col customWidth="1" max="6" min="6" style="2" width="10.42578125"/>
+    <col customWidth="1" max="9" min="7" style="8" width="8.7109375"/>
+    <col customWidth="1" max="9" min="7" style="8" width="8.7109375"/>
+    <col customWidth="1" max="9" min="7" style="8" width="8.7109375"/>
     <col customWidth="1" max="10" min="10" style="9" width="8.7109375"/>
-    <col customWidth="1" max="13" min="11" style="2" width="8.7109375"/>
-    <col customWidth="1" max="13" min="11" style="2" width="8.7109375"/>
-    <col customWidth="1" max="13" min="11" style="2" width="8.7109375"/>
+    <col customWidth="1" max="13" min="11" style="1" width="8.7109375"/>
+    <col customWidth="1" max="13" min="11" style="1" width="8.7109375"/>
+    <col customWidth="1" max="13" min="11" style="1" width="8.7109375"/>
+    <col hidden="1" max="14" min="14" style="1"/>
+    <col customWidth="1" max="15" min="15" style="4" width="46.5703125"/>
   </cols>
   <sheetData>
-    <row spans="1:13" customHeight="1" r="1" ht="30" s="2">
-      <c s="11" r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c s="11" r="B1" t="s">
+    <row customHeight="1" r="1" s="1" spans="1:15" ht="30">
+      <c r="A1" t="s" s="11">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="11">
         <v>1</v>
       </c>
-      <c s="11" r="C1" t="s">
+      <c r="C1" t="s" s="11">
         <v>2</v>
       </c>
-      <c s="11" r="D1" t="s">
+      <c r="D1" t="s" s="11">
         <v>3</v>
       </c>
-      <c s="8" r="E1" t="s">
+      <c r="E1" t="s" s="10">
         <v>4</v>
       </c>
-      <c s="8" r="F1" t="s">
+      <c r="F1" t="s" s="10">
         <v>5</v>
       </c>
-      <c s="7" r="G1" t="s">
+      <c r="G1" t="s" s="8">
         <v>6</v>
       </c>
-      <c s="7" r="I1" t="s">
+      <c r="I1" t="s" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row customFormat="1" spans="1:13" r="2" s="9">
-      <c s="4" r="F2" t="n"/>
-      <c s="7" r="G2" t="s">
+      <c r="K1" t="s" s="11">
         <v>8</v>
       </c>
-      <c s="7" r="H2" t="s">
+      <c r="L1" t="s" s="11">
         <v>9</v>
       </c>
-      <c s="7" r="I2" t="s">
+      <c r="M1" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s" s="11">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row s="9" r="2" spans="1:15" customFormat="1">
+      <c r="F2" t="n" s="3"/>
+      <c r="G2" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.716537290402336</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.06177140008272025</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.3828070650088721</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" t="n">
+        <v>12</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.01673814587599491</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3.774993734750918e-05</v>
+      </c>
+      <c r="N3" t="n">
+        <v>5.252260117075778e-12</v>
+      </c>
+      <c r="O3" t="s" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="1">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
         <v>8</v>
       </c>
-      <c s="7" r="J2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row spans="1:13" r="3" s="2">
-      <c s="9" r="A3" t="s">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.431630098954375</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0540165036827964</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.3364534011699197</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7</v>
+      </c>
+      <c r="K4" t="n">
+        <v>15</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.01681035072106541</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1.46761966487083e-05</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2.574220785623342e-13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="1">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.281063296808722</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K5" t="n">
+        <v>15</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="1">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.009133538341586</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J6" t="n">
+        <v>7</v>
+      </c>
+      <c r="K6" t="n">
+        <v>18</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="1">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.008564224330564</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7</v>
+      </c>
+      <c r="K7" t="n">
+        <v>18</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.7666222177601451</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.03024986106892207</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.2815069206441883</v>
+      </c>
+      <c r="J8" t="n">
+        <v>7</v>
+      </c>
+      <c r="K8" t="n">
+        <v>18</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.01354929806055695</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.631343958718812e-05</v>
+      </c>
+      <c r="N8" t="n">
+        <v>8.672466542022001e-16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="1">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.370975967550133</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.02237823030245666</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.3074966769446402</v>
+      </c>
+      <c r="J9" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="K9" t="n">
         <v>10</v>
       </c>
-      <c s="9" r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c s="9" r="C3" t="n">
+      <c r="L9" t="n">
+        <v>0.007520210893410571</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5.442042164499658e-05</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.804128975503948e-13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="1">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.194910513283386</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.02486360876974042</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.3095952433767538</v>
+      </c>
+      <c r="J10" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>12</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.008624965665532348</v>
+      </c>
+      <c r="M10" t="n">
+        <v>2.372849861312013e-05</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1.540944432221676e-14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="1">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="n">
         <v>1</v>
       </c>
-      <c s="9" r="D3" t="n">
+      <c r="D11" t="n">
         <v>3</v>
       </c>
-      <c s="10" r="E3" t="s">
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.90051496082524</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0122738089794267</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.2943587918480357</v>
+      </c>
+      <c r="J11" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K11" t="n">
         <v>12</v>
       </c>
-      <c s="9" r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c s="7" r="G3" t="n">
+      <c r="L11" t="n">
+        <v>0.005088371812697424</v>
+      </c>
+      <c r="M11" t="n">
+        <v>7.163879434247151e-05</v>
+      </c>
+      <c r="N11" t="n">
+        <v>2.335141161151883e-15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="1">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="n">
         <v>0.9371340888613919</v>
       </c>
-      <c s="7" r="H3" t="n">
+      <c r="H12" t="n">
         <v>0.01074846000943494</v>
       </c>
-      <c s="7" r="I3" t="n">
+      <c r="I12" t="n">
         <v>0.3102820672969054</v>
       </c>
-      <c s="7" r="J3" t="n">
+      <c r="J12" t="n">
+        <v>5</v>
+      </c>
+      <c r="K12" t="n">
+        <v>14</v>
+      </c>
+      <c r="L12" t="n">
         <v>0.004066539835950562</v>
       </c>
-    </row>
-    <row spans="1:13" r="4" s="2"/>
-    <row spans="1:13" r="5" s="2"/>
-    <row spans="1:13" r="6" s="2">
-      <c s="8" r="E6" t="n"/>
-      <c s="8" r="F6" t="n"/>
-    </row>
-    <row spans="1:13" r="7" s="2"/>
-    <row spans="1:13" r="8" s="2">
-      <c t="s" r="A8">
-        <v>10</v>
-      </c>
-      <c t="s" r="B8">
-        <v>11</v>
-      </c>
-      <c t="n" r="C8">
-        <v>1</v>
-      </c>
-      <c t="n" r="D8">
-        <v>3</v>
-      </c>
-      <c t="s" r="E8">
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2.398409482341314e-15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="1"/>
+    <row r="14" spans="1:15" s="1">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.716537290402336</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.06177140008272025</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.3828070650088721</v>
+      </c>
+      <c r="J14" t="n">
+        <v>6</v>
+      </c>
+      <c r="K14" t="n">
         <v>12</v>
       </c>
-      <c t="s" r="F8">
-        <v>13</v>
-      </c>
-      <c t="n" r="G8">
-        <v>0.9371340888613919</v>
-      </c>
-      <c t="n" r="H8">
-        <v>0.01074846000943494</v>
-      </c>
-      <c t="n" r="I8">
-        <v>0.3102820672969054</v>
-      </c>
-      <c t="n" r="J8">
-        <v>0.004066539835950562</v>
+      <c r="L14" t="n">
+        <v>0.01673814587599491</v>
+      </c>
+      <c r="M14" t="n">
+        <v>3.774993734750918e-05</v>
+      </c>
+      <c r="N14" t="n">
+        <v>5.252260117075778e-12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="1">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.771904484938687</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0569559799620466</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.3984798928781473</v>
+      </c>
+      <c r="J15" t="n">
+        <v>5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>15</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.01453746139660942</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>6.295741538494868e-12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="1">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.660363837084957</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.04977306244512677</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3657919225152383</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5</v>
+      </c>
+      <c r="K16" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.01390926153245486</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>3.235911656528066e-12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="1">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.632898984549292</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.06612585719258794</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.3575614483374006</v>
+      </c>
+      <c r="J17" t="n">
+        <v>5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.02076961521419033</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>3.513243346005982e-12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="E6:E7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>

</xml_diff>

<commit_message>
Added exp energy based cutoff function
</commit_message>
<xml_diff>
--- a/Fits/fit_results.xlsx
+++ b/Fits/fit_results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>Control File</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Fit015</t>
+  </si>
+  <si>
+    <t>Fit012</t>
+  </si>
+  <si>
+    <t>Fit016</t>
   </si>
 </sst>
 </file>
@@ -489,7 +495,7 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
@@ -514,7 +520,7 @@
     <col customWidth="1" max="15" min="15" style="4" width="46.5703125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" r="1" s="1" spans="1:15" ht="30">
+    <row r="1" ht="30" customHeight="1" spans="1:15" s="1">
       <c r="A1" t="s" s="11">
         <v>0</v>
       </c>
@@ -555,7 +561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row s="9" r="2" spans="1:15" customFormat="1">
+    <row r="2" spans="1:15" s="9" customFormat="1">
       <c r="F2" t="n" s="3"/>
       <c r="G2" t="s" s="8">
         <v>13</v>
@@ -1188,6 +1194,100 @@
       </c>
       <c r="N17" t="n">
         <v>3.513243346005982e-12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="1">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.372534128271123</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.03527432770636527</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.3165515876592619</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.009680758460240567</v>
+      </c>
+      <c r="K18" t="n">
+        <v>7</v>
+      </c>
+      <c r="L18" t="n">
+        <v>10</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.009680758460240567</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>3.449748154796696e-13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="1">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.633497756077309</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.05397988103115311</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.3573013357182082</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.01576847984847383</v>
+      </c>
+      <c r="K19" t="n">
+        <v>7</v>
+      </c>
+      <c r="L19" t="n">
+        <v>10</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.01576847984847383</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>3.044860279865397e-12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented scaling ion tof by sqrt(mass)
</commit_message>
<xml_diff>
--- a/Fits/fit_results.xlsx
+++ b/Fits/fit_results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
   <si>
     <t>Control
 File</t>
@@ -385,6 +385,33 @@
   </si>
   <si>
     <t>Fit033_4</t>
+  </si>
+  <si>
+    <t>Fit034_1</t>
+  </si>
+  <si>
+    <t>Fit034_2</t>
+  </si>
+  <si>
+    <t>Fit034_3</t>
+  </si>
+  <si>
+    <t>Fit034_4</t>
+  </si>
+  <si>
+    <t>Fit034_5</t>
+  </si>
+  <si>
+    <t>Fit034_6</t>
+  </si>
+  <si>
+    <t>Fit034_7</t>
+  </si>
+  <si>
+    <t>Knudsen H2 &amp; D2 Global:FFR ECutM ECutS Fixed:IonTOF=3.2 scaled T=299-836K t_fit=auto</t>
+  </si>
+  <si>
+    <t>Fit034_8</t>
   </si>
   <si>
     <t>D2 v0</t>
@@ -771,7 +798,7 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:R97"/>
+  <dimension ref="A1:R127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
       <pane activePane="bottomRight" state="frozen" topLeftCell="C69" xSplit="1" ySplit="2"/>
@@ -801,69 +828,69 @@
     <col hidden="1" max="18" min="18" style="16"/>
   </cols>
   <sheetData>
-    <row ht="30" customHeight="1" r="1" s="16" spans="1:18">
-      <c t="s" r="A1" s="11">
-        <v>0</v>
-      </c>
-      <c t="s" r="B1" s="13">
-        <v>1</v>
-      </c>
-      <c t="s" r="C1" s="13">
-        <v>2</v>
-      </c>
-      <c t="s" r="D1" s="13">
+    <row spans="1:18" ht="30" s="16" customHeight="1" r="1">
+      <c s="11" t="s" r="A1">
+        <v>0</v>
+      </c>
+      <c s="13" t="s" r="B1">
+        <v>1</v>
+      </c>
+      <c s="13" t="s" r="C1">
+        <v>2</v>
+      </c>
+      <c s="13" t="s" r="D1">
         <v>3</v>
       </c>
-      <c t="s" r="E1" s="11">
+      <c s="11" t="s" r="E1">
         <v>4</v>
       </c>
-      <c t="s" r="F1" s="11">
+      <c s="11" t="s" r="F1">
         <v>5</v>
       </c>
-      <c t="s" r="G1" s="15">
+      <c s="15" t="s" r="G1">
         <v>6</v>
       </c>
-      <c t="s" r="I1" s="15">
-        <v>7</v>
-      </c>
-      <c t="s" r="K1" s="13">
+      <c s="15" t="s" r="I1">
+        <v>7</v>
+      </c>
+      <c s="13" t="s" r="K1">
         <v>8</v>
       </c>
-      <c t="s" r="L1" s="13">
+      <c s="13" t="s" r="L1">
         <v>9</v>
       </c>
-      <c t="s" r="M1" s="14">
+      <c s="14" t="s" r="M1">
         <v>10</v>
       </c>
-      <c t="s" r="N1" s="14">
+      <c s="14" t="s" r="N1">
         <v>11</v>
       </c>
-      <c t="s" r="O1" s="14">
+      <c s="14" t="s" r="O1">
         <v>12</v>
       </c>
-      <c t="s" r="P1" s="11">
+      <c s="11" t="s" r="P1">
         <v>13</v>
       </c>
     </row>
-    <row customFormat="1" s="12" r="2" spans="1:18">
-      <c t="s" r="G2" s="15">
+    <row spans="1:18" customFormat="1" s="12" r="2">
+      <c s="15" t="s" r="G2">
         <v>14</v>
       </c>
-      <c t="s" r="H2" s="15">
+      <c s="15" t="s" r="H2">
         <v>15</v>
       </c>
-      <c t="s" r="I2" s="15">
+      <c s="15" t="s" r="I2">
         <v>14</v>
       </c>
-      <c t="s" r="J2" s="15">
+      <c s="15" t="s" r="J2">
         <v>15</v>
       </c>
     </row>
-    <row ht="15" customHeight="1" r="3" s="16" spans="1:18">
+    <row spans="1:18" ht="15" s="16" customHeight="1" r="3">
       <c t="s" r="A3">
         <v>16</v>
       </c>
-      <c t="s" r="B3" s="13">
+      <c s="13" t="s" r="B3">
         <v>17</v>
       </c>
       <c t="n" r="C3">
@@ -872,19 +899,19 @@
       <c t="n" r="D3">
         <v>2</v>
       </c>
-      <c t="s" r="E3" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F3" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G3" s="5">
+      <c s="12" t="s" r="E3">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F3">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G3">
         <v>1.716537290402336</v>
       </c>
-      <c t="n" r="H3" s="5">
+      <c s="5" t="n" r="H3">
         <v>0.06177140008272025</v>
       </c>
-      <c t="n" r="I3" s="5">
+      <c s="5" t="n" r="I3">
         <v>0.3828070650088721</v>
       </c>
       <c t="n" r="K3">
@@ -893,15 +920,15 @@
       <c t="n" r="L3">
         <v>12</v>
       </c>
-      <c t="s" r="P3" s="2">
+      <c s="2" t="s" r="P3">
         <v>20</v>
       </c>
     </row>
-    <row ht="15" customHeight="1" r="4" s="16" spans="1:18">
+    <row spans="1:18" ht="15" s="16" customHeight="1" r="4">
       <c t="s" r="A4">
         <v>21</v>
       </c>
-      <c t="s" r="B4" s="13">
+      <c s="13" t="s" r="B4">
         <v>17</v>
       </c>
       <c t="n" r="C4">
@@ -910,19 +937,19 @@
       <c t="n" r="D4">
         <v>8</v>
       </c>
-      <c t="s" r="E4" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F4" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G4" s="5">
+      <c s="12" t="s" r="E4">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F4">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G4">
         <v>1.431630098954375</v>
       </c>
-      <c t="n" r="H4" s="5">
+      <c s="5" t="n" r="H4">
         <v>0.0540165036827964</v>
       </c>
-      <c t="n" r="I4" s="5">
+      <c s="5" t="n" r="I4">
         <v>0.3364534011699197</v>
       </c>
       <c t="n" r="K4">
@@ -932,11 +959,11 @@
         <v>15</v>
       </c>
     </row>
-    <row s="16" r="5" spans="1:18">
+    <row spans="1:18" s="16" r="5">
       <c t="s" r="A5">
         <v>22</v>
       </c>
-      <c t="s" r="B5" s="13">
+      <c s="13" t="s" r="B5">
         <v>17</v>
       </c>
       <c t="n" r="C5">
@@ -945,19 +972,19 @@
       <c t="n" r="D5">
         <v>2</v>
       </c>
-      <c t="s" r="E5" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F5" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G5" s="5">
+      <c s="12" t="s" r="E5">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F5">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G5">
         <v>1.281063296808722</v>
       </c>
-      <c t="n" r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c t="n" r="I5" s="5">
+      <c s="5" t="n" r="H5">
+        <v>0</v>
+      </c>
+      <c s="5" t="n" r="I5">
         <v>0.4</v>
       </c>
       <c t="n" r="K5">
@@ -967,11 +994,11 @@
         <v>15</v>
       </c>
     </row>
-    <row s="16" r="6" spans="1:18">
+    <row spans="1:18" s="16" r="6">
       <c t="s" r="A6">
         <v>23</v>
       </c>
-      <c t="s" r="B6" s="13">
+      <c s="13" t="s" r="B6">
         <v>17</v>
       </c>
       <c t="n" r="C6">
@@ -980,19 +1007,19 @@
       <c t="n" r="D6">
         <v>2</v>
       </c>
-      <c t="s" r="E6" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F6" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G6" s="5">
+      <c s="12" t="s" r="E6">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F6">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G6">
         <v>1.009133538341586</v>
       </c>
-      <c t="n" r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c t="n" r="I6" s="5">
+      <c s="5" t="n" r="H6">
+        <v>0</v>
+      </c>
+      <c s="5" t="n" r="I6">
         <v>0.4</v>
       </c>
       <c t="n" r="K6">
@@ -1002,11 +1029,11 @@
         <v>18</v>
       </c>
     </row>
-    <row s="16" r="7" spans="1:18">
+    <row spans="1:18" s="16" r="7">
       <c t="s" r="A7">
         <v>24</v>
       </c>
-      <c t="s" r="B7" s="13">
+      <c s="13" t="s" r="B7">
         <v>17</v>
       </c>
       <c t="n" r="C7">
@@ -1015,19 +1042,19 @@
       <c t="n" r="D7">
         <v>2</v>
       </c>
-      <c t="s" r="E7" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F7" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G7" s="5">
+      <c s="12" t="s" r="E7">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F7">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G7">
         <v>1.008564224330564</v>
       </c>
-      <c t="n" r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c t="n" r="I7" s="5">
+      <c s="5" t="n" r="H7">
+        <v>0</v>
+      </c>
+      <c s="5" t="n" r="I7">
         <v>0.4</v>
       </c>
       <c t="n" r="K7">
@@ -1037,11 +1064,11 @@
         <v>18</v>
       </c>
     </row>
-    <row s="16" r="8" spans="1:18">
+    <row spans="1:18" s="16" r="8">
       <c t="s" r="A8">
         <v>25</v>
       </c>
-      <c t="s" r="B8" s="13">
+      <c s="13" t="s" r="B8">
         <v>17</v>
       </c>
       <c t="n" r="C8">
@@ -1050,19 +1077,19 @@
       <c t="n" r="D8">
         <v>6</v>
       </c>
-      <c t="s" r="E8" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F8" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G8" s="5">
+      <c s="12" t="s" r="E8">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F8">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G8">
         <v>0.7666222177601451</v>
       </c>
-      <c t="n" r="H8" s="5">
+      <c s="5" t="n" r="H8">
         <v>0.03024986106892207</v>
       </c>
-      <c t="n" r="I8" s="5">
+      <c s="5" t="n" r="I8">
         <v>0.2815069206441883</v>
       </c>
       <c t="n" r="K8">
@@ -1072,11 +1099,11 @@
         <v>18</v>
       </c>
     </row>
-    <row s="16" r="9" spans="1:18">
+    <row spans="1:18" s="16" r="9">
       <c t="s" r="A9">
         <v>26</v>
       </c>
-      <c t="s" r="B9" s="13">
+      <c s="13" t="s" r="B9">
         <v>27</v>
       </c>
       <c t="n" r="C9">
@@ -1085,19 +1112,19 @@
       <c t="n" r="D9">
         <v>3</v>
       </c>
-      <c t="s" r="E9" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F9" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G9" s="5">
+      <c s="12" t="s" r="E9">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F9">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G9">
         <v>1.370975967550133</v>
       </c>
-      <c t="n" r="H9" s="5">
+      <c s="5" t="n" r="H9">
         <v>0.02237823030245666</v>
       </c>
-      <c t="n" r="I9" s="5">
+      <c s="5" t="n" r="I9">
         <v>0.3074966769446402</v>
       </c>
       <c t="n" r="K9">
@@ -1107,11 +1134,11 @@
         <v>10</v>
       </c>
     </row>
-    <row s="16" r="10" spans="1:18">
+    <row spans="1:18" s="16" r="10">
       <c t="s" r="A10">
         <v>28</v>
       </c>
-      <c t="s" r="B10" s="13">
+      <c s="13" t="s" r="B10">
         <v>27</v>
       </c>
       <c t="n" r="C10">
@@ -1120,19 +1147,19 @@
       <c t="n" r="D10">
         <v>7</v>
       </c>
-      <c t="s" r="E10" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F10" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G10" s="5">
+      <c s="12" t="s" r="E10">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F10">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G10">
         <v>1.194910513283386</v>
       </c>
-      <c t="n" r="H10" s="5">
+      <c s="5" t="n" r="H10">
         <v>0.02486360876974042</v>
       </c>
-      <c t="n" r="I10" s="5">
+      <c s="5" t="n" r="I10">
         <v>0.3095952433767538</v>
       </c>
       <c t="n" r="K10">
@@ -1142,11 +1169,11 @@
         <v>12</v>
       </c>
     </row>
-    <row s="16" r="11" spans="1:18">
+    <row spans="1:18" s="16" r="11">
       <c t="s" r="A11">
         <v>29</v>
       </c>
-      <c t="s" r="B11" s="13">
+      <c s="13" t="s" r="B11">
         <v>27</v>
       </c>
       <c t="n" r="C11">
@@ -1155,19 +1182,19 @@
       <c t="n" r="D11">
         <v>3</v>
       </c>
-      <c t="s" r="E11" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F11" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G11" s="5">
+      <c s="12" t="s" r="E11">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F11">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G11">
         <v>0.90051496082524</v>
       </c>
-      <c t="n" r="H11" s="5">
+      <c s="5" t="n" r="H11">
         <v>0.0122738089794267</v>
       </c>
-      <c t="n" r="I11" s="5">
+      <c s="5" t="n" r="I11">
         <v>0.2943587918480357</v>
       </c>
       <c t="n" r="K11">
@@ -1177,11 +1204,11 @@
         <v>12</v>
       </c>
     </row>
-    <row s="16" r="12" spans="1:18">
+    <row spans="1:18" s="16" r="12">
       <c t="s" r="A12">
         <v>30</v>
       </c>
-      <c t="s" r="B12" s="13">
+      <c s="13" t="s" r="B12">
         <v>27</v>
       </c>
       <c t="n" r="C12">
@@ -1190,19 +1217,19 @@
       <c t="n" r="D12">
         <v>3</v>
       </c>
-      <c t="s" r="E12" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F12" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G12" s="5">
+      <c s="12" t="s" r="E12">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F12">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G12">
         <v>0.9371340888613919</v>
       </c>
-      <c t="n" r="H12" s="5">
+      <c s="5" t="n" r="H12">
         <v>0.01074846000943494</v>
       </c>
-      <c t="n" r="I12" s="5">
+      <c s="5" t="n" r="I12">
         <v>0.3102820672969054</v>
       </c>
       <c t="n" r="K12">
@@ -1212,11 +1239,11 @@
         <v>14</v>
       </c>
     </row>
-    <row s="16" r="13" spans="1:18">
+    <row spans="1:18" s="16" r="13">
       <c t="s" r="A13">
         <v>31</v>
       </c>
-      <c t="s" r="B13" s="13">
+      <c s="13" t="s" r="B13">
         <v>17</v>
       </c>
       <c t="n" r="C13">
@@ -1225,19 +1252,19 @@
       <c t="n" r="D13">
         <v>2</v>
       </c>
-      <c t="s" r="E13" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F13" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G13" s="5">
+      <c s="12" t="s" r="E13">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F13">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G13">
         <v>1.716537290402336</v>
       </c>
-      <c t="n" r="H13" s="5">
+      <c s="5" t="n" r="H13">
         <v>0.06177140008272025</v>
       </c>
-      <c t="n" r="I13" s="5">
+      <c s="5" t="n" r="I13">
         <v>0.3828070650088721</v>
       </c>
       <c t="n" r="K13">
@@ -1247,11 +1274,11 @@
         <v>12</v>
       </c>
     </row>
-    <row s="16" r="14" spans="1:18">
+    <row spans="1:18" s="16" r="14">
       <c t="s" r="A14">
         <v>32</v>
       </c>
-      <c t="s" r="B14" s="13">
+      <c s="13" t="s" r="B14">
         <v>17</v>
       </c>
       <c t="n" r="C14">
@@ -1260,19 +1287,19 @@
       <c t="n" r="D14">
         <v>2</v>
       </c>
-      <c t="s" r="E14" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F14" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G14" s="5">
+      <c s="12" t="s" r="E14">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F14">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G14">
         <v>1.771904484938687</v>
       </c>
-      <c t="n" r="H14" s="5">
+      <c s="5" t="n" r="H14">
         <v>0.0569559799620466</v>
       </c>
-      <c t="n" r="I14" s="5">
+      <c s="5" t="n" r="I14">
         <v>0.3984798928781473</v>
       </c>
       <c t="n" r="K14">
@@ -1282,11 +1309,11 @@
         <v>15</v>
       </c>
     </row>
-    <row s="16" r="15" spans="1:18">
+    <row spans="1:18" s="16" r="15">
       <c t="s" r="A15">
         <v>33</v>
       </c>
-      <c t="s" r="B15" s="13">
+      <c s="13" t="s" r="B15">
         <v>17</v>
       </c>
       <c t="n" r="C15">
@@ -1295,19 +1322,19 @@
       <c t="n" r="D15">
         <v>2</v>
       </c>
-      <c t="s" r="E15" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F15" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G15" s="5">
+      <c s="12" t="s" r="E15">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F15">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G15">
         <v>1.660363837084957</v>
       </c>
-      <c t="n" r="H15" s="5">
+      <c s="5" t="n" r="H15">
         <v>0.04977306244512677</v>
       </c>
-      <c t="n" r="I15" s="5">
+      <c s="5" t="n" r="I15">
         <v>0.3657919225152383</v>
       </c>
       <c t="n" r="K15">
@@ -1317,11 +1344,11 @@
         <v>10.5</v>
       </c>
     </row>
-    <row s="16" r="16" spans="1:18">
+    <row spans="1:18" s="16" r="16">
       <c t="s" r="A16">
         <v>34</v>
       </c>
-      <c t="s" r="B16" s="13">
+      <c s="13" t="s" r="B16">
         <v>17</v>
       </c>
       <c t="n" r="C16">
@@ -1330,19 +1357,19 @@
       <c t="n" r="D16">
         <v>2</v>
       </c>
-      <c t="s" r="E16" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F16" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G16" s="5">
+      <c s="12" t="s" r="E16">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F16">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G16">
         <v>1.632898984549292</v>
       </c>
-      <c t="n" r="H16" s="5">
+      <c s="5" t="n" r="H16">
         <v>0.06612585719258794</v>
       </c>
-      <c t="n" r="I16" s="5">
+      <c s="5" t="n" r="I16">
         <v>0.3575614483374006</v>
       </c>
       <c t="n" r="K16">
@@ -1352,11 +1379,11 @@
         <v>9.5</v>
       </c>
     </row>
-    <row s="16" r="17" spans="1:18">
+    <row spans="1:18" s="16" r="17">
       <c t="s" r="A17">
         <v>35</v>
       </c>
-      <c t="s" r="B17" s="13">
+      <c s="13" t="s" r="B17">
         <v>17</v>
       </c>
       <c t="n" r="C17">
@@ -1365,22 +1392,22 @@
       <c t="n" r="D17">
         <v>2</v>
       </c>
-      <c t="s" r="E17" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F17" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G17" s="5">
+      <c s="12" t="s" r="E17">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F17">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G17">
         <v>1.372534128271123</v>
       </c>
-      <c t="n" r="H17" s="5">
+      <c s="5" t="n" r="H17">
         <v>0.03527432770636527</v>
       </c>
-      <c t="n" r="I17" s="5">
+      <c s="5" t="n" r="I17">
         <v>0.3165515876592619</v>
       </c>
-      <c t="n" r="J17" s="5">
+      <c s="5" t="n" r="J17">
         <v>0.009680758460240567</v>
       </c>
       <c t="n" r="K17">
@@ -1390,11 +1417,11 @@
         <v>10</v>
       </c>
     </row>
-    <row s="16" r="18" spans="1:18">
+    <row spans="1:18" s="16" r="18">
       <c t="s" r="A18">
         <v>36</v>
       </c>
-      <c t="s" r="B18" s="13">
+      <c s="13" t="s" r="B18">
         <v>17</v>
       </c>
       <c t="n" r="C18">
@@ -1403,22 +1430,22 @@
       <c t="n" r="D18">
         <v>2</v>
       </c>
-      <c t="s" r="E18" s="12">
-        <v>18</v>
-      </c>
-      <c t="s" r="F18" s="12">
-        <v>19</v>
-      </c>
-      <c t="n" r="G18" s="5">
+      <c s="12" t="s" r="E18">
+        <v>18</v>
+      </c>
+      <c s="12" t="s" r="F18">
+        <v>19</v>
+      </c>
+      <c s="5" t="n" r="G18">
         <v>1.633497756077309</v>
       </c>
-      <c t="n" r="H18" s="5">
+      <c s="5" t="n" r="H18">
         <v>0.05397988103115311</v>
       </c>
-      <c t="n" r="I18" s="5">
+      <c s="5" t="n" r="I18">
         <v>0.3573013357182082</v>
       </c>
-      <c t="n" r="J18" s="5">
+      <c s="5" t="n" r="J18">
         <v>0.01576847984847383</v>
       </c>
       <c t="n" r="K18">
@@ -1428,19 +1455,19 @@
         <v>10</v>
       </c>
     </row>
-    <row s="16" r="19" spans="1:18">
-      <c t="n" r="E19" s="12"/>
-      <c t="n" r="F19" s="12"/>
-      <c t="n" r="G19" s="5"/>
-      <c t="n" r="H19" s="5"/>
-      <c t="n" r="I19" s="5"/>
-      <c t="n" r="J19" s="5"/>
-    </row>
-    <row s="16" r="20" spans="1:18">
+    <row spans="1:18" s="16" r="19">
+      <c s="12" t="n" r="E19"/>
+      <c s="12" t="n" r="F19"/>
+      <c s="5" t="n" r="G19"/>
+      <c s="5" t="n" r="H19"/>
+      <c s="5" t="n" r="I19"/>
+      <c s="5" t="n" r="J19"/>
+    </row>
+    <row spans="1:18" s="16" r="20">
       <c t="s" r="A20">
         <v>37</v>
       </c>
-      <c t="s" r="B20" s="12">
+      <c s="12" t="s" r="B20">
         <v>17</v>
       </c>
       <c t="n" r="C20">
@@ -1449,7 +1476,7 @@
       <c t="n" r="D20">
         <v>2</v>
       </c>
-      <c t="s" r="E20" s="12">
+      <c s="12" t="s" r="E20">
         <v>38</v>
       </c>
       <c t="s" r="F20">
@@ -1474,11 +1501,11 @@
         <v>39</v>
       </c>
     </row>
-    <row s="16" r="21" spans="1:18">
+    <row spans="1:18" s="16" r="21">
       <c t="s" r="A21">
         <v>40</v>
       </c>
-      <c t="s" r="B21" s="12">
+      <c s="12" t="s" r="B21">
         <v>17</v>
       </c>
       <c t="n" r="C21">
@@ -1487,7 +1514,7 @@
       <c t="n" r="D21">
         <v>2</v>
       </c>
-      <c t="s" r="E21" s="12">
+      <c s="12" t="s" r="E21">
         <v>38</v>
       </c>
       <c t="s" r="F21">
@@ -1512,11 +1539,11 @@
         <v>41</v>
       </c>
     </row>
-    <row s="16" r="22" spans="1:18">
+    <row spans="1:18" s="16" r="22">
       <c t="s" r="A22">
         <v>42</v>
       </c>
-      <c t="s" r="B22" s="12">
+      <c s="12" t="s" r="B22">
         <v>17</v>
       </c>
       <c t="n" r="C22">
@@ -1525,7 +1552,7 @@
       <c t="n" r="D22">
         <v>2</v>
       </c>
-      <c t="s" r="E22" s="12">
+      <c s="12" t="s" r="E22">
         <v>38</v>
       </c>
       <c t="s" r="F22">
@@ -1550,11 +1577,11 @@
         <v>43</v>
       </c>
     </row>
-    <row s="16" r="23" spans="1:18">
+    <row spans="1:18" s="16" r="23">
       <c t="s" r="A23">
         <v>44</v>
       </c>
-      <c t="s" r="B23" s="12">
+      <c s="12" t="s" r="B23">
         <v>17</v>
       </c>
       <c t="n" r="C23">
@@ -1563,7 +1590,7 @@
       <c t="n" r="D23">
         <v>2</v>
       </c>
-      <c t="s" r="E23" s="12">
+      <c s="12" t="s" r="E23">
         <v>38</v>
       </c>
       <c t="s" r="F23">
@@ -1588,12 +1615,12 @@
         <v>45</v>
       </c>
     </row>
-    <row s="16" r="24" spans="1:18"/>
-    <row s="16" r="25" spans="1:18">
+    <row spans="1:18" s="16" r="24"/>
+    <row spans="1:18" s="16" r="25">
       <c t="s" r="A25">
         <v>46</v>
       </c>
-      <c t="s" r="B25" s="12">
+      <c s="12" t="s" r="B25">
         <v>17</v>
       </c>
       <c t="n" r="C25">
@@ -1602,7 +1629,7 @@
       <c t="n" r="D25">
         <v>2</v>
       </c>
-      <c t="s" r="E25" s="12">
+      <c s="12" t="s" r="E25">
         <v>38</v>
       </c>
       <c t="s" r="F25">
@@ -1627,11 +1654,11 @@
         <v>47</v>
       </c>
     </row>
-    <row s="16" r="26" spans="1:18">
+    <row spans="1:18" s="16" r="26">
       <c t="s" r="A26">
         <v>48</v>
       </c>
-      <c t="s" r="B26" s="12">
+      <c s="12" t="s" r="B26">
         <v>17</v>
       </c>
       <c t="n" r="C26">
@@ -1640,7 +1667,7 @@
       <c t="n" r="D26">
         <v>2</v>
       </c>
-      <c t="s" r="E26" s="12">
+      <c s="12" t="s" r="E26">
         <v>38</v>
       </c>
       <c t="s" r="F26">
@@ -1665,11 +1692,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="27" spans="1:18">
+    <row spans="1:18" s="16" r="27">
       <c t="s" r="A27">
         <v>50</v>
       </c>
-      <c t="s" r="B27" s="12">
+      <c s="12" t="s" r="B27">
         <v>17</v>
       </c>
       <c t="n" r="C27">
@@ -1678,7 +1705,7 @@
       <c t="n" r="D27">
         <v>2</v>
       </c>
-      <c t="s" r="E27" s="12">
+      <c s="12" t="s" r="E27">
         <v>38</v>
       </c>
       <c t="s" r="F27">
@@ -1703,11 +1730,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="28" spans="1:18">
+    <row spans="1:18" s="16" r="28">
       <c t="s" r="A28">
         <v>51</v>
       </c>
-      <c t="s" r="B28" s="12">
+      <c s="12" t="s" r="B28">
         <v>17</v>
       </c>
       <c t="n" r="C28">
@@ -1716,7 +1743,7 @@
       <c t="n" r="D28">
         <v>2</v>
       </c>
-      <c t="s" r="E28" s="12">
+      <c s="12" t="s" r="E28">
         <v>38</v>
       </c>
       <c t="s" r="F28">
@@ -1741,12 +1768,12 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="29" spans="1:18"/>
-    <row s="16" r="30" spans="1:18">
+    <row spans="1:18" s="16" r="29"/>
+    <row spans="1:18" s="16" r="30">
       <c t="s" r="A30">
         <v>52</v>
       </c>
-      <c t="s" r="B30" s="12">
+      <c s="12" t="s" r="B30">
         <v>17</v>
       </c>
       <c t="n" r="C30">
@@ -1755,7 +1782,7 @@
       <c t="n" r="D30">
         <v>2</v>
       </c>
-      <c t="s" r="E30" s="12">
+      <c s="12" t="s" r="E30">
         <v>18</v>
       </c>
       <c t="s" r="F30">
@@ -1795,11 +1822,11 @@
         <v>54</v>
       </c>
     </row>
-    <row s="16" r="31" spans="1:18">
+    <row spans="1:18" s="16" r="31">
       <c t="s" r="A31">
         <v>55</v>
       </c>
-      <c t="s" r="B31" s="12">
+      <c s="12" t="s" r="B31">
         <v>17</v>
       </c>
       <c t="n" r="C31">
@@ -1808,7 +1835,7 @@
       <c t="n" r="D31">
         <v>2</v>
       </c>
-      <c t="s" r="E31" s="12">
+      <c s="12" t="s" r="E31">
         <v>18</v>
       </c>
       <c t="s" r="F31">
@@ -1848,11 +1875,11 @@
         <v>56</v>
       </c>
     </row>
-    <row s="16" r="32" spans="1:18">
+    <row spans="1:18" s="16" r="32">
       <c t="s" r="A32">
         <v>57</v>
       </c>
-      <c t="s" r="B32" s="12">
+      <c s="12" t="s" r="B32">
         <v>17</v>
       </c>
       <c t="n" r="C32">
@@ -1861,7 +1888,7 @@
       <c t="n" r="D32">
         <v>2</v>
       </c>
-      <c t="s" r="E32" s="12">
+      <c s="12" t="s" r="E32">
         <v>18</v>
       </c>
       <c t="s" r="F32">
@@ -1898,11 +1925,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="33" spans="1:18">
+    <row spans="1:18" s="16" r="33">
       <c t="s" r="A33">
         <v>58</v>
       </c>
-      <c t="s" r="B33" s="12">
+      <c s="12" t="s" r="B33">
         <v>17</v>
       </c>
       <c t="n" r="C33">
@@ -1911,7 +1938,7 @@
       <c t="n" r="D33">
         <v>2</v>
       </c>
-      <c t="s" r="E33" s="12">
+      <c s="12" t="s" r="E33">
         <v>18</v>
       </c>
       <c t="s" r="F33">
@@ -1948,11 +1975,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="34" spans="1:18">
+    <row spans="1:18" s="16" r="34">
       <c t="s" r="A34">
         <v>59</v>
       </c>
-      <c t="s" r="B34" s="12">
+      <c s="12" t="s" r="B34">
         <v>17</v>
       </c>
       <c t="n" r="C34">
@@ -1961,7 +1988,7 @@
       <c t="n" r="D34">
         <v>2</v>
       </c>
-      <c t="s" r="E34" s="12">
+      <c s="12" t="s" r="E34">
         <v>18</v>
       </c>
       <c t="s" r="F34">
@@ -1998,12 +2025,12 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="35" spans="1:18"/>
-    <row s="16" r="36" spans="1:18">
+    <row spans="1:18" s="16" r="35"/>
+    <row spans="1:18" s="16" r="36">
       <c t="s" r="A36">
         <v>60</v>
       </c>
-      <c t="s" r="B36" s="12">
+      <c s="12" t="s" r="B36">
         <v>17</v>
       </c>
       <c t="n" r="C36">
@@ -2012,7 +2039,7 @@
       <c t="n" r="D36">
         <v>2</v>
       </c>
-      <c t="s" r="E36" s="12">
+      <c s="12" t="s" r="E36">
         <v>18</v>
       </c>
       <c t="s" r="F36">
@@ -2049,11 +2076,11 @@
         <v>61</v>
       </c>
     </row>
-    <row s="16" r="37" spans="1:18">
+    <row spans="1:18" s="16" r="37">
       <c t="s" r="A37">
         <v>62</v>
       </c>
-      <c t="s" r="B37" s="12">
+      <c s="12" t="s" r="B37">
         <v>17</v>
       </c>
       <c t="n" r="C37">
@@ -2062,7 +2089,7 @@
       <c t="n" r="D37">
         <v>2</v>
       </c>
-      <c t="s" r="E37" s="12">
+      <c s="12" t="s" r="E37">
         <v>18</v>
       </c>
       <c t="s" r="F37">
@@ -2099,11 +2126,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="38" spans="1:18">
+    <row spans="1:18" s="16" r="38">
       <c t="s" r="A38">
         <v>63</v>
       </c>
-      <c t="s" r="B38" s="12">
+      <c s="12" t="s" r="B38">
         <v>17</v>
       </c>
       <c t="n" r="C38">
@@ -2112,7 +2139,7 @@
       <c t="n" r="D38">
         <v>2</v>
       </c>
-      <c t="s" r="E38" s="12">
+      <c s="12" t="s" r="E38">
         <v>18</v>
       </c>
       <c t="s" r="F38">
@@ -2149,11 +2176,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="39" spans="1:18">
+    <row spans="1:18" s="16" r="39">
       <c t="s" r="A39">
         <v>64</v>
       </c>
-      <c t="s" r="B39" s="12">
+      <c s="12" t="s" r="B39">
         <v>17</v>
       </c>
       <c t="n" r="C39">
@@ -2162,7 +2189,7 @@
       <c t="n" r="D39">
         <v>2</v>
       </c>
-      <c t="s" r="E39" s="12">
+      <c s="12" t="s" r="E39">
         <v>18</v>
       </c>
       <c t="s" r="F39">
@@ -2199,11 +2226,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="40" spans="1:18">
+    <row spans="1:18" s="16" r="40">
       <c t="s" r="A40">
         <v>65</v>
       </c>
-      <c t="s" r="B40" s="12">
+      <c s="12" t="s" r="B40">
         <v>17</v>
       </c>
       <c t="n" r="C40">
@@ -2212,7 +2239,7 @@
       <c t="n" r="D40">
         <v>2</v>
       </c>
-      <c t="s" r="E40" s="12">
+      <c s="12" t="s" r="E40">
         <v>18</v>
       </c>
       <c t="s" r="F40">
@@ -2249,12 +2276,12 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="41" spans="1:18"/>
-    <row s="16" r="42" spans="1:18">
+    <row spans="1:18" s="16" r="41"/>
+    <row spans="1:18" s="16" r="42">
       <c t="s" r="A42">
         <v>66</v>
       </c>
-      <c t="s" r="B42" s="12">
+      <c s="12" t="s" r="B42">
         <v>27</v>
       </c>
       <c t="n" r="C42">
@@ -2263,7 +2290,7 @@
       <c t="n" r="D42">
         <v>0</v>
       </c>
-      <c t="s" r="E42" s="12">
+      <c s="12" t="s" r="E42">
         <v>18</v>
       </c>
       <c t="s" r="F42">
@@ -2300,11 +2327,11 @@
         <v>67</v>
       </c>
     </row>
-    <row s="16" r="43" spans="1:18">
+    <row spans="1:18" s="16" r="43">
       <c t="s" r="A43">
         <v>68</v>
       </c>
-      <c t="s" r="B43" s="12">
+      <c s="12" t="s" r="B43">
         <v>27</v>
       </c>
       <c t="n" r="C43">
@@ -2313,7 +2340,7 @@
       <c t="n" r="D43">
         <v>1</v>
       </c>
-      <c t="s" r="E43" s="12">
+      <c s="12" t="s" r="E43">
         <v>18</v>
       </c>
       <c t="s" r="F43">
@@ -2350,11 +2377,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="44" spans="1:18">
+    <row spans="1:18" s="16" r="44">
       <c t="s" r="A44">
         <v>69</v>
       </c>
-      <c t="s" r="B44" s="12">
+      <c s="12" t="s" r="B44">
         <v>27</v>
       </c>
       <c t="n" r="C44">
@@ -2363,7 +2390,7 @@
       <c t="n" r="D44">
         <v>2</v>
       </c>
-      <c t="s" r="E44" s="12">
+      <c s="12" t="s" r="E44">
         <v>18</v>
       </c>
       <c t="s" r="F44">
@@ -2400,11 +2427,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="45" spans="1:18">
+    <row spans="1:18" s="16" r="45">
       <c t="s" r="A45">
         <v>70</v>
       </c>
-      <c t="s" r="B45" s="12">
+      <c s="12" t="s" r="B45">
         <v>27</v>
       </c>
       <c t="n" r="C45">
@@ -2413,7 +2440,7 @@
       <c t="n" r="D45">
         <v>3</v>
       </c>
-      <c t="s" r="E45" s="12">
+      <c s="12" t="s" r="E45">
         <v>18</v>
       </c>
       <c t="s" r="F45">
@@ -2450,11 +2477,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="46" spans="1:18">
+    <row spans="1:18" s="16" r="46">
       <c t="s" r="A46">
         <v>71</v>
       </c>
-      <c t="s" r="B46" s="12">
+      <c s="12" t="s" r="B46">
         <v>27</v>
       </c>
       <c t="n" r="C46">
@@ -2463,7 +2490,7 @@
       <c t="n" r="D46">
         <v>4</v>
       </c>
-      <c t="s" r="E46" s="12">
+      <c s="12" t="s" r="E46">
         <v>18</v>
       </c>
       <c t="s" r="F46">
@@ -2500,11 +2527,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="47" spans="1:18">
+    <row spans="1:18" s="16" r="47">
       <c t="s" r="A47">
         <v>72</v>
       </c>
-      <c t="s" r="B47" s="12">
+      <c s="12" t="s" r="B47">
         <v>27</v>
       </c>
       <c t="n" r="C47">
@@ -2513,7 +2540,7 @@
       <c t="n" r="D47">
         <v>5</v>
       </c>
-      <c t="s" r="E47" s="12">
+      <c s="12" t="s" r="E47">
         <v>18</v>
       </c>
       <c t="s" r="F47">
@@ -2550,11 +2577,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="48" spans="1:18">
+    <row spans="1:18" s="16" r="48">
       <c t="s" r="A48">
         <v>73</v>
       </c>
-      <c t="s" r="B48" s="12">
+      <c s="12" t="s" r="B48">
         <v>27</v>
       </c>
       <c t="n" r="C48">
@@ -2563,7 +2590,7 @@
       <c t="n" r="D48">
         <v>6</v>
       </c>
-      <c t="s" r="E48" s="12">
+      <c s="12" t="s" r="E48">
         <v>18</v>
       </c>
       <c t="s" r="F48">
@@ -2600,11 +2627,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="49" spans="1:18">
+    <row spans="1:18" s="16" r="49">
       <c t="s" r="A49">
         <v>74</v>
       </c>
-      <c t="s" r="B49" s="12">
+      <c s="12" t="s" r="B49">
         <v>27</v>
       </c>
       <c t="n" r="C49">
@@ -2613,7 +2640,7 @@
       <c t="n" r="D49">
         <v>7</v>
       </c>
-      <c t="s" r="E49" s="12">
+      <c s="12" t="s" r="E49">
         <v>18</v>
       </c>
       <c t="s" r="F49">
@@ -2650,12 +2677,12 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="50" spans="1:18"/>
-    <row s="16" r="51" spans="1:18">
+    <row spans="1:18" s="16" r="50"/>
+    <row spans="1:18" s="16" r="51">
       <c t="s" r="A51">
         <v>75</v>
       </c>
-      <c t="s" r="B51" s="12">
+      <c s="12" t="s" r="B51">
         <v>17</v>
       </c>
       <c t="n" r="C51">
@@ -2664,7 +2691,7 @@
       <c t="n" r="D51">
         <v>0</v>
       </c>
-      <c t="s" r="E51" s="12">
+      <c s="12" t="s" r="E51">
         <v>18</v>
       </c>
       <c t="s" r="F51">
@@ -2701,11 +2728,11 @@
         <v>76</v>
       </c>
     </row>
-    <row s="16" r="52" spans="1:18">
+    <row spans="1:18" s="16" r="52">
       <c t="s" r="A52">
         <v>77</v>
       </c>
-      <c t="s" r="B52" s="12">
+      <c s="12" t="s" r="B52">
         <v>17</v>
       </c>
       <c t="n" r="C52">
@@ -2714,7 +2741,7 @@
       <c t="n" r="D52">
         <v>1</v>
       </c>
-      <c t="s" r="E52" s="12">
+      <c s="12" t="s" r="E52">
         <v>18</v>
       </c>
       <c t="s" r="F52">
@@ -2751,11 +2778,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="53" spans="1:18">
+    <row spans="1:18" s="16" r="53">
       <c t="s" r="A53">
         <v>78</v>
       </c>
-      <c t="s" r="B53" s="12">
+      <c s="12" t="s" r="B53">
         <v>17</v>
       </c>
       <c t="n" r="C53">
@@ -2764,7 +2791,7 @@
       <c t="n" r="D53">
         <v>2</v>
       </c>
-      <c t="s" r="E53" s="12">
+      <c s="12" t="s" r="E53">
         <v>18</v>
       </c>
       <c t="s" r="F53">
@@ -2801,11 +2828,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="54" spans="1:18">
+    <row spans="1:18" s="16" r="54">
       <c t="s" r="A54">
         <v>79</v>
       </c>
-      <c t="s" r="B54" s="12">
+      <c s="12" t="s" r="B54">
         <v>17</v>
       </c>
       <c t="n" r="C54">
@@ -2814,7 +2841,7 @@
       <c t="n" r="D54">
         <v>3</v>
       </c>
-      <c t="s" r="E54" s="12">
+      <c s="12" t="s" r="E54">
         <v>18</v>
       </c>
       <c t="s" r="F54">
@@ -2851,11 +2878,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="55" spans="1:18">
+    <row spans="1:18" s="16" r="55">
       <c t="s" r="A55">
         <v>80</v>
       </c>
-      <c t="s" r="B55" s="12">
+      <c s="12" t="s" r="B55">
         <v>17</v>
       </c>
       <c t="n" r="C55">
@@ -2864,7 +2891,7 @@
       <c t="n" r="D55">
         <v>4</v>
       </c>
-      <c t="s" r="E55" s="12">
+      <c s="12" t="s" r="E55">
         <v>18</v>
       </c>
       <c t="s" r="F55">
@@ -2901,11 +2928,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="56" spans="1:18">
+    <row spans="1:18" s="16" r="56">
       <c t="s" r="A56">
         <v>81</v>
       </c>
-      <c t="s" r="B56" s="12">
+      <c s="12" t="s" r="B56">
         <v>17</v>
       </c>
       <c t="n" r="C56">
@@ -2914,7 +2941,7 @@
       <c t="n" r="D56">
         <v>5</v>
       </c>
-      <c t="s" r="E56" s="12">
+      <c s="12" t="s" r="E56">
         <v>18</v>
       </c>
       <c t="s" r="F56">
@@ -2951,11 +2978,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="57" spans="1:18">
+    <row spans="1:18" s="16" r="57">
       <c t="s" r="A57">
         <v>82</v>
       </c>
-      <c t="s" r="B57" s="12">
+      <c s="12" t="s" r="B57">
         <v>17</v>
       </c>
       <c t="n" r="C57">
@@ -2964,7 +2991,7 @@
       <c t="n" r="D57">
         <v>6</v>
       </c>
-      <c t="s" r="E57" s="12">
+      <c s="12" t="s" r="E57">
         <v>18</v>
       </c>
       <c t="s" r="F57">
@@ -3001,11 +3028,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="58" spans="1:18">
+    <row spans="1:18" s="16" r="58">
       <c t="s" r="A58">
         <v>83</v>
       </c>
-      <c t="s" r="B58" s="12">
+      <c s="12" t="s" r="B58">
         <v>17</v>
       </c>
       <c t="n" r="C58">
@@ -3014,7 +3041,7 @@
       <c t="n" r="D58">
         <v>7</v>
       </c>
-      <c t="s" r="E58" s="12">
+      <c s="12" t="s" r="E58">
         <v>18</v>
       </c>
       <c t="s" r="F58">
@@ -3051,11 +3078,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="59" spans="1:18">
+    <row spans="1:18" s="16" r="59">
       <c t="s" r="A59">
         <v>84</v>
       </c>
-      <c t="s" r="B59" s="12">
+      <c s="12" t="s" r="B59">
         <v>17</v>
       </c>
       <c t="n" r="C59">
@@ -3064,7 +3091,7 @@
       <c t="n" r="D59">
         <v>8</v>
       </c>
-      <c t="s" r="E59" s="12">
+      <c s="12" t="s" r="E59">
         <v>18</v>
       </c>
       <c t="s" r="F59">
@@ -3101,11 +3128,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="60" spans="1:18">
+    <row spans="1:18" s="16" r="60">
       <c t="s" r="A60">
         <v>85</v>
       </c>
-      <c t="s" r="B60" s="12">
+      <c s="12" t="s" r="B60">
         <v>17</v>
       </c>
       <c t="n" r="C60">
@@ -3114,7 +3141,7 @@
       <c t="n" r="D60">
         <v>9</v>
       </c>
-      <c t="s" r="E60" s="12">
+      <c s="12" t="s" r="E60">
         <v>18</v>
       </c>
       <c t="s" r="F60">
@@ -3151,11 +3178,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="61" spans="1:18">
+    <row spans="1:18" s="16" r="61">
       <c t="s" r="A61">
         <v>86</v>
       </c>
-      <c t="s" r="B61" s="12">
+      <c s="12" t="s" r="B61">
         <v>17</v>
       </c>
       <c t="n" r="C61">
@@ -3164,7 +3191,7 @@
       <c t="n" r="D61">
         <v>10</v>
       </c>
-      <c t="s" r="E61" s="12">
+      <c s="12" t="s" r="E61">
         <v>18</v>
       </c>
       <c t="s" r="F61">
@@ -3201,11 +3228,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="62" spans="1:18">
+    <row spans="1:18" s="16" r="62">
       <c t="s" r="A62">
         <v>87</v>
       </c>
-      <c t="s" r="B62" s="12">
+      <c s="12" t="s" r="B62">
         <v>17</v>
       </c>
       <c t="n" r="C62">
@@ -3214,7 +3241,7 @@
       <c t="n" r="D62">
         <v>12</v>
       </c>
-      <c t="s" r="E62" s="12">
+      <c s="12" t="s" r="E62">
         <v>18</v>
       </c>
       <c t="s" r="F62">
@@ -3251,11 +3278,11 @@
         <v>49</v>
       </c>
     </row>
-    <row s="16" r="63" spans="1:18">
-      <c t="n" r="B63" s="12"/>
-      <c t="n" r="E63" s="12"/>
-    </row>
-    <row s="16" r="64" spans="1:18">
+    <row spans="1:18" s="16" r="63">
+      <c s="12" t="n" r="B63"/>
+      <c s="12" t="n" r="E63"/>
+    </row>
+    <row spans="1:18" s="16" r="64">
       <c t="s" r="A64">
         <v>88</v>
       </c>
@@ -3293,7 +3320,7 @@
         <v>47</v>
       </c>
     </row>
-    <row s="16" r="65" spans="1:18">
+    <row spans="1:18" s="16" r="65">
       <c t="s" r="A65">
         <v>89</v>
       </c>
@@ -3328,7 +3355,7 @@
         <v>0.03733936619605598</v>
       </c>
     </row>
-    <row s="16" r="66" spans="1:18">
+    <row spans="1:18" s="16" r="66">
       <c t="s" r="A66">
         <v>90</v>
       </c>
@@ -3363,7 +3390,7 @@
         <v>0.043811662386834</v>
       </c>
     </row>
-    <row s="16" r="67" spans="1:18">
+    <row spans="1:18" s="16" r="67">
       <c t="s" r="A67">
         <v>91</v>
       </c>
@@ -3398,8 +3425,8 @@
         <v>0.04442930495679943</v>
       </c>
     </row>
-    <row s="16" r="68" spans="1:18"/>
-    <row s="16" r="69" spans="1:18">
+    <row spans="1:18" s="16" r="68"/>
+    <row spans="1:18" s="16" r="69">
       <c t="s" r="A69">
         <v>92</v>
       </c>
@@ -3449,7 +3476,7 @@
         <v>93</v>
       </c>
     </row>
-    <row s="16" r="70" spans="1:18">
+    <row spans="1:18" s="16" r="70">
       <c t="s" r="A70">
         <v>94</v>
       </c>
@@ -3496,7 +3523,7 @@
         <v>0.035</v>
       </c>
     </row>
-    <row s="16" r="71" spans="1:18">
+    <row spans="1:18" s="16" r="71">
       <c t="s" r="A71">
         <v>95</v>
       </c>
@@ -3543,7 +3570,7 @@
         <v>0.035</v>
       </c>
     </row>
-    <row s="16" r="72" spans="1:18">
+    <row spans="1:18" s="16" r="72">
       <c t="s" r="A72">
         <v>96</v>
       </c>
@@ -3590,7 +3617,7 @@
         <v>0.035</v>
       </c>
     </row>
-    <row s="16" r="73" spans="1:18">
+    <row spans="1:18" s="16" r="73">
       <c t="s" r="A73">
         <v>97</v>
       </c>
@@ -3637,8 +3664,8 @@
         <v>0.035</v>
       </c>
     </row>
-    <row s="16" r="74" spans="1:18"/>
-    <row s="16" r="75" spans="1:18">
+    <row spans="1:18" s="16" r="74"/>
+    <row spans="1:18" s="16" r="75">
       <c t="s" r="A75">
         <v>98</v>
       </c>
@@ -3688,7 +3715,7 @@
         <v>99</v>
       </c>
     </row>
-    <row s="16" r="76" spans="1:18">
+    <row spans="1:18" s="16" r="76">
       <c t="s" r="A76">
         <v>100</v>
       </c>
@@ -3735,7 +3762,7 @@
         <v>0.035</v>
       </c>
     </row>
-    <row s="16" r="77" spans="1:18">
+    <row spans="1:18" s="16" r="77">
       <c t="s" r="A77">
         <v>101</v>
       </c>
@@ -3782,7 +3809,7 @@
         <v>0.035</v>
       </c>
     </row>
-    <row s="16" r="78" spans="1:18">
+    <row spans="1:18" s="16" r="78">
       <c t="s" r="A78">
         <v>102</v>
       </c>
@@ -3829,7 +3856,7 @@
         <v>0.035</v>
       </c>
     </row>
-    <row s="16" r="79" spans="1:18">
+    <row spans="1:18" s="16" r="79">
       <c t="s" r="A79">
         <v>103</v>
       </c>
@@ -3876,8 +3903,8 @@
         <v>0.035</v>
       </c>
     </row>
-    <row s="16" r="80" spans="1:18"/>
-    <row s="16" r="81" spans="1:18">
+    <row spans="1:18" s="16" r="80"/>
+    <row spans="1:18" s="16" r="81">
       <c t="s" r="A81">
         <v>104</v>
       </c>
@@ -3927,7 +3954,7 @@
         <v>105</v>
       </c>
     </row>
-    <row s="16" r="82" spans="1:18">
+    <row spans="1:18" s="16" r="82">
       <c t="s" r="A82">
         <v>106</v>
       </c>
@@ -3977,8 +4004,8 @@
         <v>105</v>
       </c>
     </row>
-    <row s="16" r="83" spans="1:18"/>
-    <row s="16" r="84" spans="1:18">
+    <row spans="1:18" s="16" r="83"/>
+    <row spans="1:18" s="16" r="84">
       <c t="s" r="A84">
         <v>107</v>
       </c>
@@ -4016,7 +4043,7 @@
         <v>108</v>
       </c>
     </row>
-    <row s="16" r="85" spans="1:18">
+    <row spans="1:18" s="16" r="85">
       <c t="s" r="A85">
         <v>109</v>
       </c>
@@ -4051,7 +4078,7 @@
         <v>0.01568857363127024</v>
       </c>
     </row>
-    <row s="16" r="86" spans="1:18">
+    <row spans="1:18" s="16" r="86">
       <c t="s" r="A86">
         <v>110</v>
       </c>
@@ -4086,7 +4113,7 @@
         <v>0.01568857363127024</v>
       </c>
     </row>
-    <row s="16" r="87" spans="1:18">
+    <row spans="1:18" s="16" r="87">
       <c t="s" r="A87">
         <v>111</v>
       </c>
@@ -4121,8 +4148,8 @@
         <v>0.01568857363127024</v>
       </c>
     </row>
-    <row s="16" r="88" spans="1:18"/>
-    <row s="16" r="89" spans="1:18">
+    <row spans="1:18" s="16" r="88"/>
+    <row spans="1:18" s="16" r="89">
       <c t="s" r="A89">
         <v>112</v>
       </c>
@@ -4160,7 +4187,7 @@
         <v>113</v>
       </c>
     </row>
-    <row s="16" r="90" spans="1:18">
+    <row spans="1:18" s="16" r="90">
       <c t="s" r="A90">
         <v>114</v>
       </c>
@@ -4195,7 +4222,7 @@
         <v>0.01477813895803792</v>
       </c>
     </row>
-    <row s="16" r="91" spans="1:18">
+    <row spans="1:18" s="16" r="91">
       <c t="s" r="A91">
         <v>115</v>
       </c>
@@ -4230,7 +4257,7 @@
         <v>0.01477813895803792</v>
       </c>
     </row>
-    <row s="16" r="92" spans="1:18">
+    <row spans="1:18" s="16" r="92">
       <c t="s" r="A92">
         <v>116</v>
       </c>
@@ -4265,7 +4292,8 @@
         <v>0.01477813895803792</v>
       </c>
     </row>
-    <row s="16" r="94" spans="1:18">
+    <row spans="1:18" s="16" r="93"/>
+    <row spans="1:18" s="16" r="94">
       <c t="s" r="A94">
         <v>117</v>
       </c>
@@ -4303,7 +4331,7 @@
         <v>118</v>
       </c>
     </row>
-    <row s="16" r="95" spans="1:18">
+    <row spans="1:18" s="16" r="95">
       <c t="s" r="A95">
         <v>119</v>
       </c>
@@ -4338,7 +4366,7 @@
         <v>0.02704356330166448</v>
       </c>
     </row>
-    <row s="16" r="96" spans="1:18">
+    <row spans="1:18" s="16" r="96">
       <c t="s" r="A96">
         <v>120</v>
       </c>
@@ -4373,9 +4401,9 @@
         <v>0.02704356330166448</v>
       </c>
     </row>
-    <row s="16" r="97" spans="1:18">
+    <row spans="1:18" s="16" r="97">
       <c t="s" r="A97">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c t="s" r="B97">
         <v>27</v>
@@ -4406,6 +4434,995 @@
       </c>
       <c t="n" r="O97">
         <v>0.02704356330166448</v>
+      </c>
+      <c t="s" r="P97">
+        <v>118</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="98">
+      <c t="s" r="A98">
+        <v>119</v>
+      </c>
+      <c t="s" r="B98">
+        <v>27</v>
+      </c>
+      <c t="n" r="C98">
+        <v>0</v>
+      </c>
+      <c t="n" r="D98">
+        <v>1</v>
+      </c>
+      <c t="s" r="E98">
+        <v>38</v>
+      </c>
+      <c t="s" r="F98">
+        <v>19</v>
+      </c>
+      <c t="n" r="K98">
+        <v>7</v>
+      </c>
+      <c t="n" r="L98">
+        <v>30</v>
+      </c>
+      <c t="n" r="M98">
+        <v>29.0158465655809</v>
+      </c>
+      <c t="n" r="N98">
+        <v>7.460498554469358</v>
+      </c>
+      <c t="n" r="O98">
+        <v>0.02704356330166448</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="99">
+      <c t="s" r="A99">
+        <v>120</v>
+      </c>
+      <c t="s" r="B99">
+        <v>27</v>
+      </c>
+      <c t="n" r="C99">
+        <v>0</v>
+      </c>
+      <c t="n" r="D99">
+        <v>1</v>
+      </c>
+      <c t="s" r="E99">
+        <v>38</v>
+      </c>
+      <c t="s" r="F99">
+        <v>19</v>
+      </c>
+      <c t="n" r="K99">
+        <v>7</v>
+      </c>
+      <c t="n" r="L99">
+        <v>30</v>
+      </c>
+      <c t="n" r="M99">
+        <v>29.0158465655809</v>
+      </c>
+      <c t="n" r="N99">
+        <v>7.460498554469358</v>
+      </c>
+      <c t="n" r="O99">
+        <v>0.02704356330166448</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="100">
+      <c t="s" r="A100">
+        <v>121</v>
+      </c>
+      <c t="s" r="B100">
+        <v>27</v>
+      </c>
+      <c t="n" r="C100">
+        <v>0</v>
+      </c>
+      <c t="n" r="D100">
+        <v>1</v>
+      </c>
+      <c t="s" r="E100">
+        <v>38</v>
+      </c>
+      <c t="s" r="F100">
+        <v>19</v>
+      </c>
+      <c t="n" r="K100">
+        <v>7</v>
+      </c>
+      <c t="n" r="L100">
+        <v>30</v>
+      </c>
+      <c t="n" r="M100">
+        <v>29.0158465655809</v>
+      </c>
+      <c t="n" r="N100">
+        <v>7.460498554469358</v>
+      </c>
+      <c t="n" r="O100">
+        <v>0.02704356330166448</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="101"/>
+    <row spans="1:18" s="16" r="102">
+      <c t="s" r="A102">
+        <v>122</v>
+      </c>
+      <c t="s" r="B102">
+        <v>17</v>
+      </c>
+      <c t="n" r="C102">
+        <v>0</v>
+      </c>
+      <c t="n" r="D102">
+        <v>2</v>
+      </c>
+      <c t="s" r="E102">
+        <v>38</v>
+      </c>
+      <c t="s" r="F102">
+        <v>19</v>
+      </c>
+      <c t="n" r="K102">
+        <v>7</v>
+      </c>
+      <c t="n" r="L102">
+        <v>43</v>
+      </c>
+      <c t="n" r="M102">
+        <v>29.03652156667012</v>
+      </c>
+      <c t="n" r="N102">
+        <v>7.063770756022997</v>
+      </c>
+      <c t="n" r="O102">
+        <v>0.02527424663613633</v>
+      </c>
+      <c t="s" r="P102">
+        <v>118</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="103">
+      <c t="s" r="A103">
+        <v>123</v>
+      </c>
+      <c t="s" r="B103">
+        <v>27</v>
+      </c>
+      <c t="n" r="C103">
+        <v>0</v>
+      </c>
+      <c t="n" r="D103">
+        <v>1</v>
+      </c>
+      <c t="s" r="E103">
+        <v>38</v>
+      </c>
+      <c t="s" r="F103">
+        <v>19</v>
+      </c>
+      <c t="n" r="K103">
+        <v>7</v>
+      </c>
+      <c t="n" r="L103">
+        <v>43</v>
+      </c>
+      <c t="n" r="M103">
+        <v>29.03652156667012</v>
+      </c>
+      <c t="n" r="N103">
+        <v>7.063770756022997</v>
+      </c>
+      <c t="n" r="O103">
+        <v>0.02527424663613633</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="104">
+      <c t="s" r="A104">
+        <v>124</v>
+      </c>
+      <c t="s" r="B104">
+        <v>27</v>
+      </c>
+      <c t="n" r="C104">
+        <v>0</v>
+      </c>
+      <c t="n" r="D104">
+        <v>1</v>
+      </c>
+      <c t="s" r="E104">
+        <v>38</v>
+      </c>
+      <c t="s" r="F104">
+        <v>19</v>
+      </c>
+      <c t="n" r="K104">
+        <v>7</v>
+      </c>
+      <c t="n" r="L104">
+        <v>43</v>
+      </c>
+      <c t="n" r="M104">
+        <v>29.03652156667012</v>
+      </c>
+      <c t="n" r="N104">
+        <v>7.063770756022997</v>
+      </c>
+      <c t="n" r="O104">
+        <v>0.02527424663613633</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="105">
+      <c t="s" r="A105">
+        <v>125</v>
+      </c>
+      <c t="s" r="B105">
+        <v>27</v>
+      </c>
+      <c t="n" r="C105">
+        <v>0</v>
+      </c>
+      <c t="n" r="D105">
+        <v>1</v>
+      </c>
+      <c t="s" r="E105">
+        <v>38</v>
+      </c>
+      <c t="s" r="F105">
+        <v>19</v>
+      </c>
+      <c t="n" r="K105">
+        <v>7</v>
+      </c>
+      <c t="n" r="L105">
+        <v>43</v>
+      </c>
+      <c t="n" r="M105">
+        <v>29.03652156667012</v>
+      </c>
+      <c t="n" r="N105">
+        <v>7.063770756022997</v>
+      </c>
+      <c t="n" r="O105">
+        <v>0.02527424663613633</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="106">
+      <c t="s" r="A106">
+        <v>122</v>
+      </c>
+      <c t="s" r="B106">
+        <v>17</v>
+      </c>
+      <c t="n" r="C106">
+        <v>0</v>
+      </c>
+      <c t="n" r="D106">
+        <v>2</v>
+      </c>
+      <c t="s" r="E106">
+        <v>38</v>
+      </c>
+      <c t="s" r="F106">
+        <v>19</v>
+      </c>
+      <c t="n" r="K106">
+        <v>7</v>
+      </c>
+      <c t="n" r="L106">
+        <v>43</v>
+      </c>
+      <c t="n" r="M106">
+        <v>29.15517594542452</v>
+      </c>
+      <c t="n" r="N106">
+        <v>8.103531853923744</v>
+      </c>
+      <c t="n" r="O106">
+        <v>0.02455579126939211</v>
+      </c>
+      <c t="s" r="P106">
+        <v>118</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="107">
+      <c t="s" r="A107">
+        <v>123</v>
+      </c>
+      <c t="s" r="B107">
+        <v>17</v>
+      </c>
+      <c t="n" r="C107">
+        <v>0</v>
+      </c>
+      <c t="n" r="D107">
+        <v>2</v>
+      </c>
+      <c t="s" r="E107">
+        <v>38</v>
+      </c>
+      <c t="s" r="F107">
+        <v>19</v>
+      </c>
+      <c t="n" r="K107">
+        <v>7</v>
+      </c>
+      <c t="n" r="L107">
+        <v>43</v>
+      </c>
+      <c t="n" r="M107">
+        <v>29.15517594542452</v>
+      </c>
+      <c t="n" r="N107">
+        <v>8.103531853923744</v>
+      </c>
+      <c t="n" r="O107">
+        <v>0.02455579126939211</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="108">
+      <c t="s" r="A108">
+        <v>124</v>
+      </c>
+      <c t="s" r="B108">
+        <v>17</v>
+      </c>
+      <c t="n" r="C108">
+        <v>0</v>
+      </c>
+      <c t="n" r="D108">
+        <v>2</v>
+      </c>
+      <c t="s" r="E108">
+        <v>38</v>
+      </c>
+      <c t="s" r="F108">
+        <v>19</v>
+      </c>
+      <c t="n" r="K108">
+        <v>7</v>
+      </c>
+      <c t="n" r="L108">
+        <v>43</v>
+      </c>
+      <c t="n" r="M108">
+        <v>29.15517594542452</v>
+      </c>
+      <c t="n" r="N108">
+        <v>8.103531853923744</v>
+      </c>
+      <c t="n" r="O108">
+        <v>0.02455579126939211</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="109">
+      <c t="s" r="A109">
+        <v>125</v>
+      </c>
+      <c t="s" r="B109">
+        <v>17</v>
+      </c>
+      <c t="n" r="C109">
+        <v>0</v>
+      </c>
+      <c t="n" r="D109">
+        <v>2</v>
+      </c>
+      <c t="s" r="E109">
+        <v>38</v>
+      </c>
+      <c t="s" r="F109">
+        <v>19</v>
+      </c>
+      <c t="n" r="K109">
+        <v>7</v>
+      </c>
+      <c t="n" r="L109">
+        <v>43</v>
+      </c>
+      <c t="n" r="M109">
+        <v>29.15517594542452</v>
+      </c>
+      <c t="n" r="N109">
+        <v>8.103531853923744</v>
+      </c>
+      <c t="n" r="O109">
+        <v>0.02455579126939211</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="110">
+      <c t="s" r="A110">
+        <v>126</v>
+      </c>
+      <c t="s" r="B110">
+        <v>27</v>
+      </c>
+      <c t="n" r="C110">
+        <v>0</v>
+      </c>
+      <c t="n" r="D110">
+        <v>1</v>
+      </c>
+      <c t="s" r="E110">
+        <v>38</v>
+      </c>
+      <c t="s" r="F110">
+        <v>19</v>
+      </c>
+      <c t="n" r="K110">
+        <v>7</v>
+      </c>
+      <c t="n" r="L110">
+        <v>43</v>
+      </c>
+      <c t="n" r="M110">
+        <v>29.15517594542452</v>
+      </c>
+      <c t="n" r="N110">
+        <v>8.103531853923744</v>
+      </c>
+      <c t="n" r="O110">
+        <v>0.02455579126939211</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="111">
+      <c t="s" r="A111">
+        <v>127</v>
+      </c>
+      <c t="s" r="B111">
+        <v>27</v>
+      </c>
+      <c t="n" r="C111">
+        <v>0</v>
+      </c>
+      <c t="n" r="D111">
+        <v>1</v>
+      </c>
+      <c t="s" r="E111">
+        <v>38</v>
+      </c>
+      <c t="s" r="F111">
+        <v>19</v>
+      </c>
+      <c t="n" r="K111">
+        <v>7</v>
+      </c>
+      <c t="n" r="L111">
+        <v>43</v>
+      </c>
+      <c t="n" r="M111">
+        <v>29.15517594542452</v>
+      </c>
+      <c t="n" r="N111">
+        <v>8.103531853923744</v>
+      </c>
+      <c t="n" r="O111">
+        <v>0.02455579126939211</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="112">
+      <c t="s" r="A112">
+        <v>128</v>
+      </c>
+      <c t="s" r="B112">
+        <v>27</v>
+      </c>
+      <c t="n" r="C112">
+        <v>0</v>
+      </c>
+      <c t="n" r="D112">
+        <v>1</v>
+      </c>
+      <c t="s" r="E112">
+        <v>38</v>
+      </c>
+      <c t="s" r="F112">
+        <v>19</v>
+      </c>
+      <c t="n" r="K112">
+        <v>7</v>
+      </c>
+      <c t="n" r="L112">
+        <v>43</v>
+      </c>
+      <c t="n" r="M112">
+        <v>29.15517594542452</v>
+      </c>
+      <c t="n" r="N112">
+        <v>8.103531853923744</v>
+      </c>
+      <c t="n" r="O112">
+        <v>0.02455579126939211</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="113">
+      <c t="s" r="A113">
+        <v>122</v>
+      </c>
+      <c t="s" r="B113">
+        <v>17</v>
+      </c>
+      <c t="n" r="C113">
+        <v>0</v>
+      </c>
+      <c t="n" r="D113">
+        <v>2</v>
+      </c>
+      <c t="s" r="E113">
+        <v>38</v>
+      </c>
+      <c t="s" r="F113">
+        <v>19</v>
+      </c>
+      <c t="n" r="M113">
+        <v>29.13888436778263</v>
+      </c>
+      <c t="n" r="N113">
+        <v>7.669788761534208</v>
+      </c>
+      <c t="n" r="O113">
+        <v>0.02435282737568612</v>
+      </c>
+      <c t="s" r="P113">
+        <v>129</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="114">
+      <c t="s" r="A114">
+        <v>123</v>
+      </c>
+      <c t="s" r="B114">
+        <v>17</v>
+      </c>
+      <c t="n" r="C114">
+        <v>0</v>
+      </c>
+      <c t="n" r="D114">
+        <v>2</v>
+      </c>
+      <c t="s" r="E114">
+        <v>38</v>
+      </c>
+      <c t="s" r="F114">
+        <v>19</v>
+      </c>
+      <c t="n" r="M114">
+        <v>29.13888436778263</v>
+      </c>
+      <c t="n" r="N114">
+        <v>7.669788761534208</v>
+      </c>
+      <c t="n" r="O114">
+        <v>0.02435282737568612</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="115">
+      <c t="s" r="A115">
+        <v>124</v>
+      </c>
+      <c t="s" r="B115">
+        <v>17</v>
+      </c>
+      <c t="n" r="C115">
+        <v>0</v>
+      </c>
+      <c t="n" r="D115">
+        <v>2</v>
+      </c>
+      <c t="s" r="E115">
+        <v>38</v>
+      </c>
+      <c t="s" r="F115">
+        <v>19</v>
+      </c>
+      <c t="n" r="M115">
+        <v>29.13888436778263</v>
+      </c>
+      <c t="n" r="N115">
+        <v>7.669788761534208</v>
+      </c>
+      <c t="n" r="O115">
+        <v>0.02435282737568612</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="116">
+      <c t="s" r="A116">
+        <v>125</v>
+      </c>
+      <c t="s" r="B116">
+        <v>17</v>
+      </c>
+      <c t="n" r="C116">
+        <v>0</v>
+      </c>
+      <c t="n" r="D116">
+        <v>2</v>
+      </c>
+      <c t="s" r="E116">
+        <v>38</v>
+      </c>
+      <c t="s" r="F116">
+        <v>19</v>
+      </c>
+      <c t="n" r="M116">
+        <v>29.13888436778263</v>
+      </c>
+      <c t="n" r="N116">
+        <v>7.669788761534208</v>
+      </c>
+      <c t="n" r="O116">
+        <v>0.02435282737568612</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="117">
+      <c t="s" r="A117">
+        <v>126</v>
+      </c>
+      <c t="s" r="B117">
+        <v>27</v>
+      </c>
+      <c t="n" r="C117">
+        <v>0</v>
+      </c>
+      <c t="n" r="D117">
+        <v>1</v>
+      </c>
+      <c t="s" r="E117">
+        <v>38</v>
+      </c>
+      <c t="s" r="F117">
+        <v>19</v>
+      </c>
+      <c t="n" r="M117">
+        <v>29.13888436778263</v>
+      </c>
+      <c t="n" r="N117">
+        <v>7.669788761534208</v>
+      </c>
+      <c t="n" r="O117">
+        <v>0.02435282737568612</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="118">
+      <c t="s" r="A118">
+        <v>127</v>
+      </c>
+      <c t="s" r="B118">
+        <v>27</v>
+      </c>
+      <c t="n" r="C118">
+        <v>0</v>
+      </c>
+      <c t="n" r="D118">
+        <v>1</v>
+      </c>
+      <c t="s" r="E118">
+        <v>38</v>
+      </c>
+      <c t="s" r="F118">
+        <v>19</v>
+      </c>
+      <c t="n" r="M118">
+        <v>29.13888436778263</v>
+      </c>
+      <c t="n" r="N118">
+        <v>7.669788761534208</v>
+      </c>
+      <c t="n" r="O118">
+        <v>0.02435282737568612</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="119">
+      <c t="s" r="A119">
+        <v>128</v>
+      </c>
+      <c t="s" r="B119">
+        <v>27</v>
+      </c>
+      <c t="n" r="C119">
+        <v>0</v>
+      </c>
+      <c t="n" r="D119">
+        <v>1</v>
+      </c>
+      <c t="s" r="E119">
+        <v>38</v>
+      </c>
+      <c t="s" r="F119">
+        <v>19</v>
+      </c>
+      <c t="n" r="M119">
+        <v>29.13888436778263</v>
+      </c>
+      <c t="n" r="N119">
+        <v>7.669788761534208</v>
+      </c>
+      <c t="n" r="O119">
+        <v>0.02435282737568612</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="120">
+      <c t="s" r="A120">
+        <v>122</v>
+      </c>
+      <c t="s" r="B120">
+        <v>17</v>
+      </c>
+      <c t="n" r="C120">
+        <v>0</v>
+      </c>
+      <c t="n" r="D120">
+        <v>2</v>
+      </c>
+      <c t="s" r="E120">
+        <v>38</v>
+      </c>
+      <c t="s" r="F120">
+        <v>19</v>
+      </c>
+      <c t="n" r="K120">
+        <v>7</v>
+      </c>
+      <c t="n" r="L120">
+        <v>40</v>
+      </c>
+      <c t="n" r="M120">
+        <v>29.13621885391749</v>
+      </c>
+      <c t="n" r="N120">
+        <v>7.004997155345219</v>
+      </c>
+      <c t="n" r="O120">
+        <v>0.02370315598203582</v>
+      </c>
+      <c t="s" r="P120">
+        <v>129</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="121">
+      <c t="s" r="A121">
+        <v>123</v>
+      </c>
+      <c t="s" r="B121">
+        <v>17</v>
+      </c>
+      <c t="n" r="C121">
+        <v>0</v>
+      </c>
+      <c t="n" r="D121">
+        <v>2</v>
+      </c>
+      <c t="s" r="E121">
+        <v>38</v>
+      </c>
+      <c t="s" r="F121">
+        <v>19</v>
+      </c>
+      <c t="n" r="K121">
+        <v>7</v>
+      </c>
+      <c t="n" r="L121">
+        <v>40</v>
+      </c>
+      <c t="n" r="M121">
+        <v>29.13621885391749</v>
+      </c>
+      <c t="n" r="N121">
+        <v>7.004997155345219</v>
+      </c>
+      <c t="n" r="O121">
+        <v>0.02370315598203582</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="122">
+      <c t="s" r="A122">
+        <v>124</v>
+      </c>
+      <c t="s" r="B122">
+        <v>17</v>
+      </c>
+      <c t="n" r="C122">
+        <v>0</v>
+      </c>
+      <c t="n" r="D122">
+        <v>2</v>
+      </c>
+      <c t="s" r="E122">
+        <v>38</v>
+      </c>
+      <c t="s" r="F122">
+        <v>19</v>
+      </c>
+      <c t="n" r="K122">
+        <v>7</v>
+      </c>
+      <c t="n" r="L122">
+        <v>40</v>
+      </c>
+      <c t="n" r="M122">
+        <v>29.13621885391749</v>
+      </c>
+      <c t="n" r="N122">
+        <v>7.004997155345219</v>
+      </c>
+      <c t="n" r="O122">
+        <v>0.02370315598203582</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="123">
+      <c t="s" r="A123">
+        <v>125</v>
+      </c>
+      <c t="s" r="B123">
+        <v>17</v>
+      </c>
+      <c t="n" r="C123">
+        <v>0</v>
+      </c>
+      <c t="n" r="D123">
+        <v>2</v>
+      </c>
+      <c t="s" r="E123">
+        <v>38</v>
+      </c>
+      <c t="s" r="F123">
+        <v>19</v>
+      </c>
+      <c t="n" r="K123">
+        <v>7</v>
+      </c>
+      <c t="n" r="L123">
+        <v>40</v>
+      </c>
+      <c t="n" r="M123">
+        <v>29.13621885391749</v>
+      </c>
+      <c t="n" r="N123">
+        <v>7.004997155345219</v>
+      </c>
+      <c t="n" r="O123">
+        <v>0.02370315598203582</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="124">
+      <c t="s" r="A124">
+        <v>126</v>
+      </c>
+      <c t="s" r="B124">
+        <v>27</v>
+      </c>
+      <c t="n" r="C124">
+        <v>0</v>
+      </c>
+      <c t="n" r="D124">
+        <v>1</v>
+      </c>
+      <c t="s" r="E124">
+        <v>38</v>
+      </c>
+      <c t="s" r="F124">
+        <v>19</v>
+      </c>
+      <c t="n" r="K124">
+        <v>7</v>
+      </c>
+      <c t="n" r="L124">
+        <v>40</v>
+      </c>
+      <c t="n" r="M124">
+        <v>29.13621885391749</v>
+      </c>
+      <c t="n" r="N124">
+        <v>7.004997155345219</v>
+      </c>
+      <c t="n" r="O124">
+        <v>0.02370315598203582</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="125">
+      <c t="s" r="A125">
+        <v>127</v>
+      </c>
+      <c t="s" r="B125">
+        <v>27</v>
+      </c>
+      <c t="n" r="C125">
+        <v>0</v>
+      </c>
+      <c t="n" r="D125">
+        <v>1</v>
+      </c>
+      <c t="s" r="E125">
+        <v>38</v>
+      </c>
+      <c t="s" r="F125">
+        <v>19</v>
+      </c>
+      <c t="n" r="K125">
+        <v>7</v>
+      </c>
+      <c t="n" r="L125">
+        <v>40</v>
+      </c>
+      <c t="n" r="M125">
+        <v>29.13621885391749</v>
+      </c>
+      <c t="n" r="N125">
+        <v>7.004997155345219</v>
+      </c>
+      <c t="n" r="O125">
+        <v>0.02370315598203582</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="126">
+      <c t="s" r="A126">
+        <v>128</v>
+      </c>
+      <c t="s" r="B126">
+        <v>27</v>
+      </c>
+      <c t="n" r="C126">
+        <v>0</v>
+      </c>
+      <c t="n" r="D126">
+        <v>1</v>
+      </c>
+      <c t="s" r="E126">
+        <v>38</v>
+      </c>
+      <c t="s" r="F126">
+        <v>19</v>
+      </c>
+      <c t="n" r="K126">
+        <v>7</v>
+      </c>
+      <c t="n" r="L126">
+        <v>40</v>
+      </c>
+      <c t="n" r="M126">
+        <v>29.13621885391749</v>
+      </c>
+      <c t="n" r="N126">
+        <v>7.004997155345219</v>
+      </c>
+      <c t="n" r="O126">
+        <v>0.02370315598203582</v>
+      </c>
+    </row>
+    <row spans="1:18" s="16" r="127">
+      <c t="s" r="A127">
+        <v>130</v>
+      </c>
+      <c t="s" r="B127">
+        <v>27</v>
+      </c>
+      <c t="n" r="C127">
+        <v>0</v>
+      </c>
+      <c t="n" r="D127">
+        <v>1</v>
+      </c>
+      <c t="s" r="E127">
+        <v>38</v>
+      </c>
+      <c t="s" r="F127">
+        <v>19</v>
+      </c>
+      <c t="n" r="K127">
+        <v>7</v>
+      </c>
+      <c t="n" r="L127">
+        <v>40</v>
+      </c>
+      <c t="n" r="M127">
+        <v>29.13621885391749</v>
+      </c>
+      <c t="n" r="N127">
+        <v>7.004997155345219</v>
+      </c>
+      <c t="n" r="O127">
+        <v>0.02370315598203582</v>
       </c>
     </row>
   </sheetData>
@@ -4452,7 +5469,7 @@
     <col hidden="1" max="7" min="6" style="16"/>
   </cols>
   <sheetData>
-    <row s="16" r="4" spans="1:7">
+    <row spans="1:7" s="16" r="4">
       <c t="n" r="F4">
         <v>0</v>
       </c>
@@ -4460,9 +5477,9 @@
         <v>0.9539342346605403</v>
       </c>
     </row>
-    <row s="16" r="5" spans="1:7">
-      <c t="s" r="A5" s="12">
-        <v>122</v>
+    <row spans="1:7" s="16" r="5">
+      <c s="12" t="s" r="A5">
+        <v>131</v>
       </c>
       <c t="n" r="F5">
         <v>1</v>
@@ -4471,13 +5488,13 @@
         <v>0.9553151110619933</v>
       </c>
     </row>
-    <row s="16" r="6" spans="1:7">
-      <c t="s" r="A6" s="6">
+    <row spans="1:7" s="16" r="6">
+      <c s="6" t="s" r="A6">
         <v>3</v>
       </c>
-      <c t="n" r="B6" s="6"/>
-      <c t="n" r="C6" s="6"/>
-      <c t="s" r="D6" s="6">
+      <c s="6" t="n" r="B6"/>
+      <c s="6" t="n" r="C6"/>
+      <c s="6" t="s" r="D6">
         <v>6</v>
       </c>
       <c t="n" r="F6">
@@ -4487,7 +5504,7 @@
         <v>0.9541183663461318</v>
       </c>
     </row>
-    <row s="16" r="7" spans="1:7">
+    <row spans="1:7" s="16" r="7">
       <c t="n" r="A7">
         <v>0</v>
       </c>
@@ -4507,7 +5524,7 @@
         <v>0.9529447036739171</v>
       </c>
     </row>
-    <row s="16" r="8" spans="1:7">
+    <row spans="1:7" s="16" r="8">
       <c t="n" r="A8">
         <v>1</v>
       </c>
@@ -4527,7 +5544,7 @@
         <v>0.9253394110363898</v>
       </c>
     </row>
-    <row s="16" r="9" spans="1:7">
+    <row spans="1:7" s="16" r="9">
       <c t="n" r="A9">
         <v>2</v>
       </c>
@@ -4547,7 +5564,7 @@
         <v>0.9091073580544464</v>
       </c>
     </row>
-    <row s="16" r="10" spans="1:7">
+    <row spans="1:7" s="16" r="10">
       <c t="n" r="A10">
         <v>3</v>
       </c>
@@ -4567,7 +5584,7 @@
         <v>0.8783324259727529</v>
       </c>
     </row>
-    <row s="16" r="11" spans="1:7">
+    <row spans="1:7" s="16" r="11">
       <c t="n" r="A11">
         <v>4</v>
       </c>
@@ -4587,7 +5604,7 @@
         <v>0.8568390193010809</v>
       </c>
     </row>
-    <row s="16" r="12" spans="1:7">
+    <row spans="1:7" s="16" r="12">
       <c t="n" r="A12">
         <v>5</v>
       </c>
@@ -4601,7 +5618,7 @@
         <v>1.496979982616633</v>
       </c>
     </row>
-    <row s="16" r="13" spans="1:7">
+    <row spans="1:7" s="16" r="13">
       <c t="n" r="A13">
         <v>6</v>
       </c>
@@ -4615,7 +5632,7 @@
         <v>1.488961839524425</v>
       </c>
     </row>
-    <row s="16" r="14" spans="1:7">
+    <row spans="1:7" s="16" r="14">
       <c t="n" r="A14">
         <v>7</v>
       </c>
@@ -4629,7 +5646,7 @@
         <v>1.448366741386381</v>
       </c>
     </row>
-    <row s="16" r="15" spans="1:7">
+    <row spans="1:7" s="16" r="15">
       <c t="n" r="A15">
         <v>8</v>
       </c>
@@ -4637,7 +5654,7 @@
         <v>1.400322532665015</v>
       </c>
     </row>
-    <row s="16" r="16" spans="1:7">
+    <row spans="1:7" s="16" r="16">
       <c t="n" r="A16">
         <v>9</v>
       </c>
@@ -4645,7 +5662,7 @@
         <v>1.393331768576858</v>
       </c>
     </row>
-    <row s="16" r="17" spans="1:7">
+    <row spans="1:7" s="16" r="17">
       <c t="n" r="A17">
         <v>10</v>
       </c>
@@ -4653,7 +5670,7 @@
         <v>1.285314329402959</v>
       </c>
     </row>
-    <row s="16" r="18" spans="1:7">
+    <row spans="1:7" s="16" r="18">
       <c t="n" r="A18">
         <v>12</v>
       </c>
@@ -4661,7 +5678,7 @@
         <v>1.172607542014761</v>
       </c>
     </row>
-    <row s="16" r="20" spans="1:7">
+    <row spans="1:7" s="16" r="20">
       <c t="n" r="F20">
         <v>0</v>
       </c>
@@ -4669,7 +5686,7 @@
         <v>1.553824532109104</v>
       </c>
     </row>
-    <row s="16" r="21" spans="1:7">
+    <row spans="1:7" s="16" r="21">
       <c t="n" r="F21">
         <v>1</v>
       </c>
@@ -4677,9 +5694,9 @@
         <v>1.54856571072677</v>
       </c>
     </row>
-    <row s="16" r="22" spans="1:7">
-      <c t="s" r="A22" s="12">
-        <v>123</v>
+    <row spans="1:7" s="16" r="22">
+      <c s="12" t="s" r="A22">
+        <v>132</v>
       </c>
       <c t="n" r="F22">
         <v>2</v>
@@ -4688,13 +5705,13 @@
         <v>1.533806136340885</v>
       </c>
     </row>
-    <row s="16" r="23" spans="1:7">
-      <c t="s" r="A23" s="6">
+    <row spans="1:7" s="16" r="23">
+      <c s="6" t="s" r="A23">
         <v>3</v>
       </c>
-      <c t="n" r="B23" s="6"/>
-      <c t="n" r="C23" s="6"/>
-      <c t="s" r="D23" s="6">
+      <c s="6" t="n" r="B23"/>
+      <c s="6" t="n" r="C23"/>
+      <c s="6" t="s" r="D23">
         <v>6</v>
       </c>
       <c t="n" r="F23">
@@ -4704,7 +5721,7 @@
         <v>1.517244828722738</v>
       </c>
     </row>
-    <row s="16" r="24" spans="1:7">
+    <row spans="1:7" s="16" r="24">
       <c t="n" r="A24">
         <v>0</v>
       </c>
@@ -4721,7 +5738,7 @@
         <v>1.482306145156003</v>
       </c>
     </row>
-    <row s="16" r="25" spans="1:7">
+    <row spans="1:7" s="16" r="25">
       <c t="n" r="A25">
         <v>1</v>
       </c>
@@ -4738,7 +5755,7 @@
         <v>1.496979982616633</v>
       </c>
     </row>
-    <row s="16" r="26" spans="1:7">
+    <row spans="1:7" s="16" r="26">
       <c t="n" r="A26">
         <v>2</v>
       </c>
@@ -4755,7 +5772,7 @@
         <v>1.488961839524425</v>
       </c>
     </row>
-    <row s="16" r="27" spans="1:7">
+    <row spans="1:7" s="16" r="27">
       <c t="n" r="A27">
         <v>3</v>
       </c>
@@ -4772,7 +5789,7 @@
         <v>1.448366741386381</v>
       </c>
     </row>
-    <row s="16" r="28" spans="1:7">
+    <row spans="1:7" s="16" r="28">
       <c t="n" r="A28">
         <v>4</v>
       </c>
@@ -4789,7 +5806,7 @@
         <v>1.400322532665015</v>
       </c>
     </row>
-    <row s="16" r="29" spans="1:7">
+    <row spans="1:7" s="16" r="29">
       <c t="n" r="A29">
         <v>5</v>
       </c>
@@ -4806,7 +5823,7 @@
         <v>1.393331768576858</v>
       </c>
     </row>
-    <row s="16" r="30" spans="1:7">
+    <row spans="1:7" s="16" r="30">
       <c t="n" r="A30">
         <v>6</v>
       </c>
@@ -4823,7 +5840,7 @@
         <v>1.285314329402959</v>
       </c>
     </row>
-    <row s="16" r="31" spans="1:7">
+    <row spans="1:7" s="16" r="31">
       <c t="n" r="A31">
         <v>7</v>
       </c>

</xml_diff>